<commit_message>
synchronized noteboks a bit
</commit_message>
<xml_diff>
--- a/ProjectTime.xlsx
+++ b/ProjectTime.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Haniff\Documents\GeneralProgramming\Diversified_Projects\AllPicker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1EBE19A-976D-478C-9F15-93F80C6AE891}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F84EE571-00BB-43C2-8D9F-D0A3A4999658}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="26083" windowHeight="10963" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="17">
   <si>
     <t>Project</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>FlaskMegaTut</t>
+  </si>
+  <si>
+    <t>Octoparse</t>
   </si>
 </sst>
 </file>
@@ -443,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C54"/>
+  <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1050,6 +1053,22 @@
         <v>2.0833333333333333E-3</v>
       </c>
     </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>15</v>
+      </c>
+      <c r="B55" s="6">
+        <v>43378</v>
+      </c>
+      <c r="C55" s="5">
+        <v>3.4722222222222224E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:C15">
     <sortCondition descending="1" ref="C2:C15"/>

</xml_diff>